<commit_message>
replace sales sales by store type
</commit_message>
<xml_diff>
--- a/visual/sample-data/pie-donut-chart/Retail Sales by Store Type.xlsx
+++ b/visual/sample-data/pie-donut-chart/Retail Sales by Store Type.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammad.syafiq\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arifah.azura\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
     <t>Footwear</t>
   </si>
   <si>
-    <t>Sales This Category</t>
+    <t>Sales</t>
   </si>
 </sst>
 </file>
@@ -410,11 +410,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>